<commit_message>
load from excel - with electives
</commit_message>
<xml_diff>
--- a/Faculty Assignment.xlsx
+++ b/Faculty Assignment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="131">
   <si>
     <t xml:space="preserve">SUBJECT CODE</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">FACULTY</t>
   </si>
   <si>
-    <t xml:space="preserve">SECTION</t>
-  </si>
-  <si>
     <t xml:space="preserve">16CS301</t>
   </si>
   <si>
@@ -58,18 +55,6 @@
     <t xml:space="preserve">Maths Faculty</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
     <t xml:space="preserve">16CS302</t>
   </si>
   <si>
@@ -271,36 +256,39 @@
     <t xml:space="preserve">Advanced Unix Programming</t>
   </si>
   <si>
-    <t xml:space="preserve">ELE-1</t>
+    <t xml:space="preserve">ELE-1, AUP</t>
   </si>
   <si>
     <t xml:space="preserve">Divya Jennifer D'Souza</t>
   </si>
   <si>
+    <t xml:space="preserve">15CS515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operations Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELE-1, OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vijay Murari T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pawan Hegde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15IL001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employability Skill Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESD</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">15CS515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operations Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vijay Murari T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pawan Hegde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15IL001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employability Skill Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microprocessors and Peripherals Lab</t>
   </si>
   <si>
@@ -391,12 +379,18 @@
     <t xml:space="preserve">Advanced Web Techniques</t>
   </si>
   <si>
+    <t xml:space="preserve">ELE-1, AWT</t>
+  </si>
+  <si>
     <t xml:space="preserve">14CS711</t>
   </si>
   <si>
     <t xml:space="preserve">Machine Learning</t>
   </si>
   <si>
+    <t xml:space="preserve">ELE-1, ML</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sarika Hegde</t>
   </si>
   <si>
@@ -406,7 +400,7 @@
     <t xml:space="preserve">Mobile Application Development</t>
   </si>
   <si>
-    <t xml:space="preserve">ELE-2</t>
+    <t xml:space="preserve">ELE-2, MAD</t>
   </si>
   <si>
     <t xml:space="preserve">Ankitha A Nayak</t>
@@ -416,6 +410,9 @@
   </si>
   <si>
     <t xml:space="preserve">Image Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELE-2, IP</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
     <tableColumn id="4" name="CREDITS"/>
     <tableColumn id="5" name="SEMESTER"/>
     <tableColumn id="6" name="FACULTY"/>
-    <tableColumn id="7" name="SECTION"/>
+    <tableColumn id="7" name=""/>
   </tableColumns>
 </table>
 </file>
@@ -548,21 +545,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.9336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,29 +582,23 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,10 +608,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,10 +618,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,1081 +628,802 @@
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F24" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F48" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F49" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F51" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F52" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F53" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C55" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F57" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G58" s="0" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F60" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G60" s="0" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G65" s="0" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G68" s="0" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F72" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G72" s="0" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F73" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G73" s="0" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G74" s="0" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F75" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G75" s="0" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F76" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G76" s="0" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F77" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G78" s="0" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F79" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G79" s="0" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F80" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G81" s="0" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F83" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F85" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G85" s="0" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F87" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G87" s="0" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F88" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F88" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G88" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F89" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G89" s="0" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B90" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>128</v>
-      </c>
       <c r="E90" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G90" s="0" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F91" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G91" s="0" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F92" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G92" s="0" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F93" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G93" s="0" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F94" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G94" s="0" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>128</v>
-      </c>
       <c r="E95" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G95" s="0" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>